<commit_message>
I'm workin'g on it
</commit_message>
<xml_diff>
--- a/Synthèse.xlsx
+++ b/Synthèse.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Radionucléide" sheetId="3" r:id="rId1"/>
     <sheet name="Param_CT_RT" sheetId="1" r:id="rId2"/>
     <sheet name="NRD_Radio" sheetId="2" r:id="rId3"/>
     <sheet name="NRD_MN" sheetId="4" r:id="rId4"/>
+    <sheet name="Param_Acq_MN" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Tension (kV)</t>
   </si>
@@ -127,6 +128,48 @@
   </si>
   <si>
     <t>Sein</t>
+  </si>
+  <si>
+    <t>Matrice</t>
+  </si>
+  <si>
+    <t>Mode Acquisition</t>
+  </si>
+  <si>
+    <t>Critère d'arrête</t>
+  </si>
+  <si>
+    <t>Nombre de coups (kcp)</t>
+  </si>
+  <si>
+    <t>Durée (s)</t>
+  </si>
+  <si>
+    <t>Fenêtre spectrométrique</t>
+  </si>
+  <si>
+    <t>Contrôle</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Intrinséque</t>
+  </si>
+  <si>
+    <t>Uniformité de réponse du système</t>
+  </si>
+  <si>
+    <t>Linéarité spatiale</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>Résolution Intrinséque en Energie</t>
+  </si>
+  <si>
+    <t>Réglementation</t>
   </si>
 </sst>
 </file>
@@ -170,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -191,6 +234,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -851,7 +903,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
@@ -864,4 +916,101 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="4" max="5" width="18.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:7" s="9" customFormat="1">
+      <c r="B4" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" s="2" customFormat="1" ht="45">
+      <c r="B5" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" s="2" customFormat="1">
+      <c r="B6" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="10"/>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="8"/>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="8"/>
+    </row>
+    <row r="9" spans="2:7" ht="30">
+      <c r="B9" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="8"/>
+      <c r="C10" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ajout CQ intrinseque gamma cam
</commit_message>
<xml_diff>
--- a/Synthèse.xlsx
+++ b/Synthèse.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="71">
   <si>
     <t>Tension (kV)</t>
   </si>
@@ -145,9 +145,6 @@
     <t>Durée (s)</t>
   </si>
   <si>
-    <t>Fenêtre spectrométrique</t>
-  </si>
-  <si>
     <t>Contrôle</t>
   </si>
   <si>
@@ -170,13 +167,126 @@
   </si>
   <si>
     <t>Réglementation</t>
+  </si>
+  <si>
+    <t>ANSM</t>
+  </si>
+  <si>
+    <t>ANSM/SFPM</t>
+  </si>
+  <si>
+    <t>Périodicité</t>
+  </si>
+  <si>
+    <t>Tolérance</t>
+  </si>
+  <si>
+    <t>- Aucun défaut ou structure particulière visible sur l'image
+-Variation &lt;2% par rapport au CQ Initial</t>
+  </si>
+  <si>
+    <t>- Aucune distortion spatiale visible</t>
+  </si>
+  <si>
+    <t>- Intial
+- Après chaque intervention ayant un impact sur le paramètre</t>
+  </si>
+  <si>
+    <t>- Initial
+- Annuel
+- Après chaque intervention qui impact le paramètre</t>
+  </si>
+  <si>
+    <t>- Initial
+- Semestriel
+- Après chaque intervention qui impact sur le paramètre</t>
+  </si>
+  <si>
+    <t>- Conforme au spec constructeur</t>
+  </si>
+  <si>
+    <t>- Ecart entre pic d'aborption tot mesuré et théorique &lt; 3 keV
+- Indice de résolution en E &lt; 12%</t>
+  </si>
+  <si>
+    <t>40 000</t>
+  </si>
+  <si>
+    <t>140 ± 10%</t>
+  </si>
+  <si>
+    <t>Fenêtre spectrométrique (keV)</t>
+  </si>
+  <si>
+    <t>Exemple pour une gamma Cam GE D670</t>
+  </si>
+  <si>
+    <t>Statique</t>
+  </si>
+  <si>
+    <t>12 000</t>
+  </si>
+  <si>
+    <t>Méthode</t>
+  </si>
+  <si>
+    <t>- Non unif intégrale
+Ui(%)= 100 x (Vmax-Vmin)/(Vmax+Vmin)
+- Non uniformité Différentielle
+Ud=Max(Udi)
+Udi(%)= 100 x (VMax-Vmin)/(VMax-Vmin)
+Ui(%) = 100 x (VMax-Vmin)/(VM+Vm)
+sur des groupes de 5 pixels</t>
+  </si>
+  <si>
+    <t>Analyse visuelle de l'image d'une mire 4 quadrants</t>
+  </si>
+  <si>
+    <t>Source ponctuelle 99mTc
+Re(%)= 100 xLMH(keV)/E(keV)</t>
+  </si>
+  <si>
+    <r>
+      <t>Analyse quantitative image mire 4 quadrant
+LMH=1,058.L.Racine(ln(&lt;ROI&gt;/racine(s</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-&lt;ROI&gt;)))</t>
+    </r>
+  </si>
+  <si>
+    <t>Mode Planaire</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -192,16 +302,63 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -209,11 +366,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -224,27 +410,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="15">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -920,93 +1163,235 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:G11"/>
+  <dimension ref="B1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:C6"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" customWidth="1"/>
-    <col min="4" max="5" width="18.5" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="15"/>
+    <col min="2" max="2" width="16.5" style="15" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="37" style="15" customWidth="1"/>
+    <col min="5" max="5" width="19" style="15" customWidth="1"/>
+    <col min="6" max="6" width="42.33203125" style="15" customWidth="1"/>
+    <col min="7" max="7" width="29.1640625" style="15" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="15"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:7" s="9" customFormat="1">
-      <c r="B4" s="9" t="s">
+    <row r="1" spans="2:8">
+      <c r="B1" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="14"/>
+    </row>
+    <row r="4" spans="2:8" s="16" customFormat="1">
+      <c r="B4" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" s="17" customFormat="1" ht="30">
+      <c r="B5" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="13" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" s="2" customFormat="1" ht="45">
-      <c r="B5" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="G5" s="2" t="s">
+    </row>
+    <row r="6" spans="2:8" s="17" customFormat="1">
+      <c r="B6" s="9" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" s="2" customFormat="1">
-      <c r="B6" s="10" t="s">
+      <c r="C6" s="9"/>
+      <c r="D6" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="10"/>
-    </row>
-    <row r="7" spans="2:7">
-      <c r="B7" s="8" t="s">
+      <c r="G6" s="18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" s="17" customFormat="1" ht="75">
+      <c r="B7" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" s="21" customFormat="1" ht="45">
+      <c r="B8" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" s="21" customFormat="1" ht="105">
+      <c r="B9" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" s="24" customFormat="1">
+      <c r="B10" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="8"/>
-    </row>
-    <row r="8" spans="2:7">
-      <c r="B8" s="8" t="s">
+      <c r="C10" s="8"/>
+      <c r="D10" s="22">
+        <v>512</v>
+      </c>
+      <c r="E10" s="22">
+        <v>512</v>
+      </c>
+      <c r="F10" s="22">
+        <v>512</v>
+      </c>
+      <c r="G10" s="23"/>
+    </row>
+    <row r="11" spans="2:8" s="24" customFormat="1">
+      <c r="B11" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="8"/>
-    </row>
-    <row r="9" spans="2:7" ht="30">
-      <c r="B9" s="8" t="s">
+      <c r="C11" s="8"/>
+      <c r="D11" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" s="24" customFormat="1" ht="30">
+      <c r="B12" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C12" s="10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="2:7">
-      <c r="B10" s="8"/>
-      <c r="C10" s="9" t="s">
+      <c r="D12" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" s="23"/>
+    </row>
+    <row r="13" spans="2:8" s="24" customFormat="1">
+      <c r="B13" s="8"/>
+      <c r="C13" s="11" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="2:7">
-      <c r="B11" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="8"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" s="24" customFormat="1">
+      <c r="B14" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B9:B10"/>
+  <mergeCells count="12">
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
ajout partie CQ mode planaire gamma cam
</commit_message>
<xml_diff>
--- a/Synthèse.xlsx
+++ b/Synthèse.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="97">
   <si>
     <t>Tension (kV)</t>
   </si>
@@ -274,12 +274,109 @@
   <si>
     <t>Mode Planaire</t>
   </si>
+  <si>
+    <t>Test visuel:
+non uniformité
+spectrométrie
+taux de comptage</t>
+  </si>
+  <si>
+    <t>Résolution spatiale</t>
+  </si>
+  <si>
+    <t>Sensibilité</t>
+  </si>
+  <si>
+    <t>SFPM</t>
+  </si>
+  <si>
+    <t>Quotidien</t>
+  </si>
+  <si>
+    <t>- A reception
+- Annuel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - A récéption</t>
+  </si>
+  <si>
+    <t>- Initial
+- Mensuel
+- Après chaque intervention qui impact le paramètre</t>
+  </si>
+  <si>
+    <t>Aucun défaut ou structure particuliére visible sur les images de contrôle</t>
+  </si>
+  <si>
+    <t>Aucune distortion spatiale ne doit être visible</t>
+  </si>
+  <si>
+    <t>RS à 10 cm ne doit pas être supérieur à 5% de la spec constructeur en X et en Y</t>
+  </si>
+  <si>
+    <t>- Ecart msr et valeur constructeur &lt; 5%
+- ecart entre les 2 détecteurs &lt; 2%</t>
+  </si>
+  <si>
+    <t>- Aucun défaut ou structure particulière sur l'image
+- variation par rapport au CQ initial &lt; 2%</t>
+  </si>
+  <si>
+    <t>Collimateur</t>
+  </si>
+  <si>
+    <t>LEHR</t>
+  </si>
+  <si>
+    <t>4 000</t>
+  </si>
+  <si>
+    <t>122 ± 10%</t>
+  </si>
+  <si>
+    <t>Radionucléïde</t>
+  </si>
+  <si>
+    <t>Co57</t>
+  </si>
+  <si>
+    <t>Tc99m</t>
+  </si>
+  <si>
+    <t>Acq avec toutes les corrections
+Détecteur en mode H
+Source plane de Co57 à 10 cm des 2 détecteurs
+Analyse visuelle</t>
+  </si>
+  <si>
+    <t>Analyse Visuelle
+Calcul des unif intégrale et unif différentielle (même methodologie qu'en intrinsèque)</t>
+  </si>
+  <si>
+    <t>Ligne source de Tc 99m
+placé au centre de la table
+RS pour plusieurs distance source détecteur
+5 cm, 10 cm, 25 cm, 20 cm, 25 cm
+mesure LMH et LDH</t>
+  </si>
+  <si>
+    <t>Stattique</t>
+  </si>
+  <si>
+    <t>Tc 99m</t>
+  </si>
+  <si>
+    <t>Boite de pétrie contenant source de Tc 99m
+acquisition pour les 2 detecteurs à différentes distance
+Calcul de l'activité moy dans boite de pétri (prise en compte de la décroissance entre la préparation de la boite et l'acq + décroissance pendant acq)
+Sensib= (Sm-Sbdf)/Amoy</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -298,6 +395,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -325,8 +429,13 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -357,8 +466,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -381,25 +502,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -420,6 +581,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -443,9 +607,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -472,8 +633,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="29">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -481,6 +666,13 @@
     <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -488,6 +680,13 @@
     <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1163,71 +1362,91 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H14"/>
+  <dimension ref="B1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="15"/>
-    <col min="2" max="2" width="16.5" style="15" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" style="15" customWidth="1"/>
-    <col min="4" max="4" width="37" style="15" customWidth="1"/>
-    <col min="5" max="5" width="19" style="15" customWidth="1"/>
-    <col min="6" max="6" width="42.33203125" style="15" customWidth="1"/>
-    <col min="7" max="7" width="29.1640625" style="15" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="15"/>
+    <col min="1" max="1" width="10.83203125" style="16"/>
+    <col min="2" max="2" width="16.5" style="16" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" style="16" customWidth="1"/>
+    <col min="4" max="4" width="37" style="16" customWidth="1"/>
+    <col min="5" max="5" width="19" style="16" customWidth="1"/>
+    <col min="6" max="6" width="42.33203125" style="16" customWidth="1"/>
+    <col min="7" max="7" width="29.1640625" style="16" customWidth="1"/>
+    <col min="8" max="12" width="25.5" style="16" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8">
-      <c r="B1" s="14" t="s">
+    <row r="1" spans="2:12">
+      <c r="B1" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="14"/>
-    </row>
-    <row r="4" spans="2:8" s="16" customFormat="1">
-      <c r="B4" s="8" t="s">
+      <c r="C1" s="15"/>
+    </row>
+    <row r="4" spans="2:12" s="4" customFormat="1">
+      <c r="B4" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="12" t="s">
+      <c r="C4" s="9"/>
+      <c r="D4" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="16" t="s">
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="26" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" s="17" customFormat="1" ht="30">
-      <c r="B5" s="9" t="s">
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+    </row>
+    <row r="5" spans="2:12" s="8" customFormat="1" ht="60">
+      <c r="B5" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="13" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="14" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" s="17" customFormat="1">
-      <c r="B6" s="9" t="s">
+      <c r="H5" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="K5" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="L5" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" s="17" customFormat="1">
+      <c r="B6" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="9"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="18" t="s">
         <v>49</v>
       </c>
@@ -1240,12 +1459,27 @@
       <c r="G6" s="18" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" s="17" customFormat="1" ht="75">
-      <c r="B7" s="9" t="s">
+      <c r="H6" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="L6" s="18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" s="17" customFormat="1" ht="75">
+      <c r="B7" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="9"/>
+      <c r="C7" s="10"/>
       <c r="D7" s="19" t="s">
         <v>54</v>
       </c>
@@ -1258,12 +1492,27 @@
       <c r="G7" s="19" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" s="21" customFormat="1" ht="45">
-      <c r="B8" s="9" t="s">
+      <c r="H7" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="K7" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="L7" s="19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" s="21" customFormat="1" ht="60">
+      <c r="B8" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="9"/>
+      <c r="C8" s="10"/>
       <c r="D8" s="20" t="s">
         <v>52</v>
       </c>
@@ -1276,12 +1525,27 @@
       <c r="G8" s="20" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" s="21" customFormat="1" ht="105">
-      <c r="B9" s="9" t="s">
+      <c r="H8" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="J8" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" s="21" customFormat="1" ht="180">
+      <c r="B9" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C9" s="9"/>
+      <c r="C9" s="10"/>
       <c r="D9" s="20" t="s">
         <v>66</v>
       </c>
@@ -1294,12 +1558,25 @@
       <c r="G9" s="20" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" s="24" customFormat="1">
-      <c r="B10" s="8" t="s">
+      <c r="H9" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="K9" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="L9" s="28" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" s="24" customFormat="1">
+      <c r="B10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="8"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="22">
         <v>512</v>
       </c>
@@ -1310,85 +1587,209 @@
         <v>512</v>
       </c>
       <c r="G10" s="23"/>
-    </row>
-    <row r="11" spans="2:8" s="24" customFormat="1">
-      <c r="B11" s="8" t="s">
+      <c r="H10" s="22">
+        <v>256</v>
+      </c>
+      <c r="I10" s="22">
+        <v>256</v>
+      </c>
+      <c r="J10" s="22">
+        <v>1024</v>
+      </c>
+      <c r="K10" s="22">
+        <v>256</v>
+      </c>
+      <c r="L10" s="22">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" s="24" customFormat="1">
+      <c r="B11" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="31"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="I11" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="J11" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="K11" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="L11" s="22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" s="24" customFormat="1">
+      <c r="B12" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="31"/>
+      <c r="D12" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="G12" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="I12" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="J12" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="K12" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="L12" s="22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" s="24" customFormat="1">
+      <c r="B13" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="22" t="s">
+      <c r="C13" s="9"/>
+      <c r="D13" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E13" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F13" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="22" t="s">
+      <c r="G13" s="22" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" s="24" customFormat="1" ht="30">
-      <c r="B12" s="8" t="s">
+      <c r="H13" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="I13" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="K13" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="L13" s="22"/>
+    </row>
+    <row r="14" spans="2:12" s="24" customFormat="1" ht="30">
+      <c r="B14" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C14" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D14" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E14" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F14" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="23"/>
-    </row>
-    <row r="13" spans="2:8" s="24" customFormat="1">
-      <c r="B13" s="8"/>
-      <c r="C13" s="11" t="s">
+      <c r="G14" s="23"/>
+      <c r="H14" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="I14" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" s="24" customFormat="1">
+      <c r="B15" s="9"/>
+      <c r="C15" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="22">
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="22">
         <v>100</v>
       </c>
-    </row>
-    <row r="14" spans="2:8" s="24" customFormat="1">
-      <c r="B14" s="8" t="s">
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="22">
+        <v>100</v>
+      </c>
+      <c r="K15" s="22">
+        <v>100</v>
+      </c>
+      <c r="L15" s="22"/>
+    </row>
+    <row r="16" spans="2:12" s="24" customFormat="1">
+      <c r="B16" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="22" t="s">
+      <c r="C16" s="9"/>
+      <c r="D16" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E16" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="F14" s="22" t="s">
+      <c r="F16" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="G14" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="I16" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="J16" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="K16" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="L16" s="22" t="s">
+        <v>87</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="15">
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="H4:L4"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:C16"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
ajout CQ planaire pour de vrai
</commit_message>
<xml_diff>
--- a/Synthèse.xlsx
+++ b/Synthèse.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="98">
   <si>
     <t>Tension (kV)</t>
   </si>
@@ -370,6 +370,10 @@
 acquisition pour les 2 detecteurs à différentes distance
 Calcul de l'activité moy dans boite de pétri (prise en compte de la décroissance entre la préparation de la boite et l'acq + décroissance pendant acq)
 Sensib= (Sm-Sbdf)/Amoy</t>
+  </si>
+  <si>
+    <t>Mire 4 quadrants positionnée sur le détecteur
+Puis Galette de Co57</t>
   </si>
 </sst>
 </file>
@@ -1365,10 +1369,10 @@
   <dimension ref="B1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="K7" sqref="K7"/>
+      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1561,7 +1565,9 @@
       <c r="H9" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="I9" s="28"/>
+      <c r="I9" s="28" t="s">
+        <v>97</v>
+      </c>
       <c r="J9" s="28" t="s">
         <v>93</v>
       </c>
@@ -1591,7 +1597,7 @@
         <v>256</v>
       </c>
       <c r="I10" s="22">
-        <v>256</v>
+        <v>512</v>
       </c>
       <c r="J10" s="22">
         <v>1024</v>
@@ -1740,7 +1746,7 @@
       <c r="K15" s="22">
         <v>100</v>
       </c>
-      <c r="L15" s="22"/>
+      <c r="L15" s="23"/>
     </row>
     <row r="16" spans="2:12" s="24" customFormat="1">
       <c r="B16" s="9" t="s">

</xml_diff>

<commit_message>
ajout CQ tomo gamma
</commit_message>
<xml_diff>
--- a/Synthèse.xlsx
+++ b/Synthèse.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="127">
   <si>
     <t>Tension (kV)</t>
   </si>
@@ -195,11 +195,6 @@
     <t>- Initial
 - Annuel
 - Après chaque intervention qui impact le paramètre</t>
-  </si>
-  <si>
-    <t>- Initial
-- Semestriel
-- Après chaque intervention qui impact sur le paramètre</t>
   </si>
   <si>
     <t>- Conforme au spec constructeur</t>
@@ -374,6 +369,119 @@
   <si>
     <t>Mire 4 quadrants positionnée sur le détecteur
 Puis Galette de Co57</t>
+  </si>
+  <si>
+    <t>Mode Tomographique</t>
+  </si>
+  <si>
+    <t>Determination du centre de rotation</t>
+  </si>
+  <si>
+    <t>Vérification de la taille du pixel</t>
+  </si>
+  <si>
+    <t>Vérification de l'exactitude angulaire</t>
+  </si>
+  <si>
+    <t>Evaluation de la variation anglaire de la spectrométrie</t>
+  </si>
+  <si>
+    <t>QI</t>
+  </si>
+  <si>
+    <t>- Mensuel les 3 premier mois
+- Mensuel ou semestriel (selon stabilité du système)</t>
+  </si>
+  <si>
+    <t>± 0,5 mm (spec constructeur)</t>
+  </si>
+  <si>
+    <t>- Initial
+- Semestrielle
+- Après chaque intervention qui impact sur le paramètre</t>
+  </si>
+  <si>
+    <t>- A la reception
+-Annuel</t>
+  </si>
+  <si>
+    <t>- Initial
+- Annuel</t>
+  </si>
+  <si>
+    <t>- Initial</t>
+  </si>
+  <si>
+    <t>- Initial
+- Après chaque intervention qui impact le paramètre</t>
+  </si>
+  <si>
+    <t>- Annuel
+- Après chaque intervention qui impact le paramètre</t>
+  </si>
+  <si>
+    <t>RS du mode tomo ne doit pas s'écarter de plus de 10% de la RS du mode planaire</t>
+  </si>
+  <si>
+    <t>Ecart max msr entre valeurs extrème
+&lt; 3 kev (ANSM)
+&lt; 2 keV (SFPM)</t>
+  </si>
+  <si>
+    <t>LEHR/MEGP/HEGP</t>
+  </si>
+  <si>
+    <t>Tomo</t>
+  </si>
+  <si>
+    <t>Utilisation du synogramme pour calculer les décalages transverses (X et Y) et le décalage axial (selon l'axe Z (TP patient))</t>
+  </si>
+  <si>
+    <t>A partir de l'acquisition de la résolution spatiale
+distances entre les lignes sources connues
+Taille pixel= (distance entre 2 lignes/Nb pixel entre 2 ligne)</t>
+  </si>
+  <si>
+    <t>25 s par projection
+120 projections
+réalisées dans le sens horaire</t>
+  </si>
+  <si>
+    <t>10 s par pas d'acquisition
+1 acquisition tous les 6° sur 720° réalisation des acquisition dans le sens horraire</t>
+  </si>
+  <si>
+    <t>Contrôle non réalisé.</t>
+  </si>
+  <si>
+    <t>LMH(centrale, tangentielle , radiale) de profil de lignes de Tc 99m disposées en 3 points sur des axes orthogonaux
+pour 2 distance 15 cm et 20 cm</t>
+  </si>
+  <si>
+    <t>Tc 99m (74 MBq)</t>
+  </si>
+  <si>
+    <t>Tc 99m (75 MBq)</t>
+  </si>
+  <si>
+    <t>Acquisition d'un spectre tous les 45° sur 360°</t>
+  </si>
+  <si>
+    <t>140 ± 20%
+et
+120 ± 10%</t>
+  </si>
+  <si>
+    <t>15 s / projection
+30 projections /détecteur</t>
+  </si>
+  <si>
+    <t>Acquisition d'un fantôme QI adaptés à la MN (Jaszszak).
+Analyse visuelle
+Analyse quantitative:
+Contraste
+Bruit
+…</t>
   </si>
 </sst>
 </file>
@@ -439,7 +547,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -479,6 +587,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -533,7 +647,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -563,8 +677,36 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -611,6 +753,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -661,8 +806,23 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="57">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -677,6 +837,20 @@
     <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -691,6 +865,20 @@
     <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1366,13 +1554,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L16"/>
+  <dimension ref="B1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="O6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomRight" activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1385,16 +1573,18 @@
     <col min="6" max="6" width="42.33203125" style="16" customWidth="1"/>
     <col min="7" max="7" width="29.1640625" style="16" customWidth="1"/>
     <col min="8" max="12" width="25.5" style="16" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="16"/>
+    <col min="13" max="17" width="21.5" style="16" customWidth="1"/>
+    <col min="18" max="18" width="22.33203125" style="16" customWidth="1"/>
+    <col min="19" max="16384" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12">
+    <row r="1" spans="2:18">
       <c r="B1" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" s="15"/>
     </row>
-    <row r="4" spans="2:12" s="4" customFormat="1">
+    <row r="4" spans="2:18" s="4" customFormat="1">
       <c r="B4" s="9" t="s">
         <v>41</v>
       </c>
@@ -1405,15 +1595,23 @@
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
-      <c r="H4" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-    </row>
-    <row r="5" spans="2:12" s="8" customFormat="1" ht="60">
+      <c r="H4" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="N4" s="35"/>
+      <c r="O4" s="35"/>
+      <c r="P4" s="35"/>
+      <c r="Q4" s="35"/>
+      <c r="R4" s="35"/>
+    </row>
+    <row r="5" spans="2:18" s="8" customFormat="1" ht="60">
       <c r="B5" s="10" t="s">
         <v>40</v>
       </c>
@@ -1430,357 +1628,534 @@
       <c r="G5" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="H5" s="27" t="s">
+      <c r="H5" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="I5" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="I5" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="J5" s="27" t="s">
+      <c r="K5" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="K5" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="L5" s="27" t="s">
+      <c r="L5" s="28" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" spans="2:12" s="17" customFormat="1">
+      <c r="M5" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="N5" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="O5" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="P5" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q5" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="R5" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" s="18" customFormat="1">
       <c r="B6" s="10" t="s">
         <v>47</v>
       </c>
       <c r="C6" s="10"/>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="K6" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="L6" s="18" t="s">
+      <c r="J6" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="L6" s="19" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="7" spans="2:12" s="17" customFormat="1" ht="75">
+      <c r="M6" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="N6" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="O6" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="P6" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q6" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="R6" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" s="18" customFormat="1" ht="75">
       <c r="B7" s="10" t="s">
         <v>50</v>
       </c>
       <c r="C7" s="10"/>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="G7" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="H7" s="18" t="s">
+      <c r="G7" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="H7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="I7" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="J7" s="19" t="s">
+      <c r="K7" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="L7" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="L7" s="19" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" s="21" customFormat="1" ht="60">
+      <c r="M7" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="N7" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="O7" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="P7" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q7" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="R7" s="20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" s="22" customFormat="1" ht="60">
       <c r="B8" s="10" t="s">
         <v>51</v>
       </c>
       <c r="C8" s="10"/>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="G8" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="H8" s="29" t="s">
+      <c r="H8" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="I8" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="I8" s="28" t="s">
+      <c r="J8" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="J8" s="28" t="s">
+      <c r="K8" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="K8" s="20" t="s">
+      <c r="L8" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="L8" s="20" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" s="21" customFormat="1" ht="180">
+      <c r="M8" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="N8" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="O8" s="38"/>
+      <c r="P8" s="38"/>
+      <c r="Q8" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="R8" s="38"/>
+    </row>
+    <row r="9" spans="2:18" s="22" customFormat="1" ht="127" customHeight="1">
       <c r="B9" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="20" t="s">
+      <c r="E9" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="F9" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="H9" s="28" t="s">
+      <c r="H9" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="I9" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="J9" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="K9" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="L9" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="I9" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="J9" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="K9" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="L9" s="28" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" s="24" customFormat="1">
+      <c r="M9" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="N9" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="O9" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="P9" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q9" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="R9" s="29" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" s="25" customFormat="1">
       <c r="B10" s="9" t="s">
         <v>35</v>
       </c>
       <c r="C10" s="9"/>
-      <c r="D10" s="22">
+      <c r="D10" s="23">
         <v>512</v>
       </c>
-      <c r="E10" s="22">
+      <c r="E10" s="23">
         <v>512</v>
       </c>
-      <c r="F10" s="22">
+      <c r="F10" s="23">
         <v>512</v>
       </c>
-      <c r="G10" s="23"/>
-      <c r="H10" s="22">
+      <c r="G10" s="24"/>
+      <c r="H10" s="23">
         <v>256</v>
       </c>
-      <c r="I10" s="22">
+      <c r="I10" s="23">
         <v>512</v>
       </c>
-      <c r="J10" s="22">
+      <c r="J10" s="23">
         <v>1024</v>
       </c>
-      <c r="K10" s="22">
+      <c r="K10" s="23">
         <v>256</v>
       </c>
-      <c r="L10" s="22">
+      <c r="L10" s="23">
         <v>512</v>
       </c>
-    </row>
-    <row r="11" spans="2:12" s="24" customFormat="1">
-      <c r="B11" s="30" t="s">
+      <c r="M10" s="23">
+        <v>256</v>
+      </c>
+      <c r="N10" s="23">
+        <v>256</v>
+      </c>
+      <c r="O10" s="23">
+        <v>256</v>
+      </c>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="23">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" s="25" customFormat="1">
+      <c r="B11" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="32"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="I11" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="J11" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="K11" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="L11" s="22" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" s="24" customFormat="1">
-      <c r="B12" s="30" t="s">
+      <c r="I11" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="J11" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="K11" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="L11" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="M11" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="N11" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="O11" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="23" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" s="25" customFormat="1">
+      <c r="B12" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" s="32"/>
+      <c r="D12" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="G12" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="H12" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="C12" s="31"/>
-      <c r="D12" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="E12" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="F12" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="G12" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="H12" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="I12" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="J12" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="K12" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="L12" s="22" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" s="24" customFormat="1">
+      <c r="I12" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="J12" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="K12" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="L12" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="M12" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N12" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="O12" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="R12" s="23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" s="25" customFormat="1">
       <c r="B13" s="9" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="9"/>
-      <c r="D13" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="F13" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="G13" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="H13" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="I13" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="J13" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="K13" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="L13" s="22"/>
-    </row>
-    <row r="14" spans="2:12" s="24" customFormat="1" ht="30">
+      <c r="D13" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="I13" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="J13" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="K13" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="N13" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="O13" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="P13" s="24"/>
+      <c r="Q13" s="24"/>
+      <c r="R13" s="23" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" s="25" customFormat="1" ht="30">
       <c r="B14" s="9" t="s">
         <v>37</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="F14" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="G14" s="23"/>
-      <c r="H14" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="I14" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="22" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" s="24" customFormat="1">
+      <c r="D14" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="24"/>
+      <c r="H14" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="24"/>
+    </row>
+    <row r="15" spans="2:18" s="17" customFormat="1" ht="90">
       <c r="B15" s="9"/>
       <c r="C15" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="22">
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="26">
         <v>100</v>
       </c>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="22">
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="26">
         <v>100</v>
       </c>
-      <c r="K15" s="22">
+      <c r="K15" s="26">
         <v>100</v>
       </c>
-      <c r="L15" s="23"/>
-    </row>
-    <row r="16" spans="2:12" s="24" customFormat="1">
+      <c r="L15" s="39"/>
+      <c r="M15" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="N15" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="O15" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="P15" s="39"/>
+      <c r="Q15" s="39"/>
+      <c r="R15" s="19" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" s="17" customFormat="1" ht="45">
       <c r="B16" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C16" s="9"/>
-      <c r="D16" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="F16" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="G16" s="23"/>
-      <c r="H16" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="I16" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="J16" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="K16" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="L16" s="22" t="s">
-        <v>87</v>
+      <c r="D16" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" s="39"/>
+      <c r="H16" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="I16" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="J16" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="K16" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="L16" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="M16" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="N16" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="O16" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="P16" s="39"/>
+      <c r="Q16" s="39"/>
+      <c r="R16" s="19" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="M4:R4"/>
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B1:C1"/>

</xml_diff>

<commit_message>
changement du nom d'un onglet
changement de "param acq MN" en "MN_CQ_Gamma_cam"
</commit_message>
<xml_diff>
--- a/Synthèse.xlsx
+++ b/Synthèse.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Param_CT_RT" sheetId="1" r:id="rId2"/>
     <sheet name="NRD_Radio" sheetId="2" r:id="rId3"/>
     <sheet name="NRD_MN" sheetId="4" r:id="rId4"/>
-    <sheet name="Param_Acq_MN" sheetId="5" r:id="rId5"/>
+    <sheet name="MN_CQ_Gamma_cam" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -488,14 +488,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -649,62 +642,62 @@
   </borders>
   <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -717,39 +710,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -782,10 +763,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -794,22 +772,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -819,6 +788,30 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1560,620 +1553,619 @@
       <pane xSplit="3" ySplit="5" topLeftCell="O6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="R10" sqref="R10"/>
+      <selection pane="bottomRight" activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="16"/>
-    <col min="2" max="2" width="16.5" style="16" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" style="16" customWidth="1"/>
-    <col min="4" max="4" width="37" style="16" customWidth="1"/>
-    <col min="5" max="5" width="19" style="16" customWidth="1"/>
-    <col min="6" max="6" width="42.33203125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="29.1640625" style="16" customWidth="1"/>
-    <col min="8" max="12" width="25.5" style="16" customWidth="1"/>
-    <col min="13" max="17" width="21.5" style="16" customWidth="1"/>
-    <col min="18" max="18" width="22.33203125" style="16" customWidth="1"/>
-    <col min="19" max="16384" width="10.83203125" style="16"/>
+    <col min="1" max="1" width="10.83203125" style="12"/>
+    <col min="2" max="2" width="16.5" style="12" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="37" style="12" customWidth="1"/>
+    <col min="5" max="5" width="19" style="12" customWidth="1"/>
+    <col min="6" max="6" width="42.33203125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="29.1640625" style="12" customWidth="1"/>
+    <col min="8" max="12" width="25.5" style="12" customWidth="1"/>
+    <col min="13" max="17" width="21.5" style="12" customWidth="1"/>
+    <col min="18" max="18" width="22.33203125" style="12" customWidth="1"/>
+    <col min="19" max="16384" width="10.83203125" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:18">
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="15"/>
+      <c r="C1" s="35"/>
     </row>
     <row r="4" spans="2:18" s="4" customFormat="1">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="13" t="s">
+      <c r="C4" s="34"/>
+      <c r="D4" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="27" t="s">
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="35" t="s">
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="35"/>
-      <c r="R4" s="35"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="32"/>
     </row>
     <row r="5" spans="2:18" s="8" customFormat="1" ht="60">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="14" t="s">
+      <c r="C5" s="36"/>
+      <c r="D5" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="I5" s="28" t="s">
+      <c r="I5" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="J5" s="28" t="s">
+      <c r="J5" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="K5" s="28" t="s">
+      <c r="K5" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="L5" s="28" t="s">
+      <c r="L5" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="M5" s="36" t="s">
+      <c r="M5" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="N5" s="36" t="s">
+      <c r="N5" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="O5" s="36" t="s">
+      <c r="O5" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="P5" s="36" t="s">
+      <c r="P5" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="Q5" s="36" t="s">
+      <c r="Q5" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="R5" s="36" t="s">
+      <c r="R5" s="28" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="2:18" s="18" customFormat="1">
-      <c r="B6" s="10" t="s">
+    <row r="6" spans="2:18" s="14" customFormat="1">
+      <c r="B6" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="19" t="s">
+      <c r="C6" s="36"/>
+      <c r="D6" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="H6" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="J6" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="K6" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="L6" s="19" t="s">
+      <c r="L6" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="M6" s="19" t="s">
+      <c r="M6" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="N6" s="19" t="s">
+      <c r="N6" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="O6" s="19" t="s">
+      <c r="O6" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="P6" s="19" t="s">
+      <c r="P6" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="Q6" s="19" t="s">
+      <c r="Q6" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="R6" s="19" t="s">
+      <c r="R6" s="15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="2:18" s="18" customFormat="1" ht="75">
-      <c r="B7" s="10" t="s">
+    <row r="7" spans="2:18" s="14" customFormat="1" ht="75">
+      <c r="B7" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="20" t="s">
+      <c r="C7" s="36"/>
+      <c r="D7" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="H7" s="37" t="s">
+      <c r="H7" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="I7" s="20" t="s">
+      <c r="I7" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="J7" s="20" t="s">
+      <c r="J7" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="K7" s="20" t="s">
+      <c r="K7" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="L7" s="20" t="s">
+      <c r="L7" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="M7" s="20" t="s">
+      <c r="M7" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="N7" s="20" t="s">
+      <c r="N7" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="O7" s="20" t="s">
+      <c r="O7" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="P7" s="20" t="s">
+      <c r="P7" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="Q7" s="20" t="s">
+      <c r="Q7" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="R7" s="20" t="s">
+      <c r="R7" s="16" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="2:18" s="22" customFormat="1" ht="60">
-      <c r="B8" s="10" t="s">
+    <row r="8" spans="2:18" s="18" customFormat="1" ht="60">
+      <c r="B8" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="21" t="s">
+      <c r="C8" s="36"/>
+      <c r="D8" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G8" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="I8" s="29" t="s">
+      <c r="I8" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="J8" s="29" t="s">
+      <c r="J8" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="K8" s="21" t="s">
+      <c r="K8" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="L8" s="21" t="s">
+      <c r="L8" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="M8" s="29" t="s">
+      <c r="M8" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="N8" s="29" t="s">
+      <c r="N8" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="O8" s="38"/>
-      <c r="P8" s="38"/>
-      <c r="Q8" s="29" t="s">
+      <c r="O8" s="30"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="R8" s="38"/>
-    </row>
-    <row r="9" spans="2:18" s="22" customFormat="1" ht="127" customHeight="1">
-      <c r="B9" s="10" t="s">
+      <c r="R8" s="30"/>
+    </row>
+    <row r="9" spans="2:18" s="18" customFormat="1" ht="127" customHeight="1">
+      <c r="B9" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="21" t="s">
+      <c r="C9" s="36"/>
+      <c r="D9" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="G9" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="29" t="s">
+      <c r="H9" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="I9" s="29" t="s">
+      <c r="I9" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="J9" s="29" t="s">
+      <c r="J9" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="K9" s="29" t="s">
+      <c r="K9" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="L9" s="29" t="s">
+      <c r="L9" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="M9" s="29" t="s">
+      <c r="M9" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="N9" s="29" t="s">
+      <c r="N9" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="O9" s="29" t="s">
+      <c r="O9" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="P9" s="29" t="s">
+      <c r="P9" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="Q9" s="29" t="s">
+      <c r="Q9" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="R9" s="29" t="s">
+      <c r="R9" s="24" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="10" spans="2:18" s="25" customFormat="1">
-      <c r="B10" s="9" t="s">
+    <row r="10" spans="2:18" s="21" customFormat="1">
+      <c r="B10" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="23">
+      <c r="C10" s="34"/>
+      <c r="D10" s="19">
         <v>512</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="19">
         <v>512</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10" s="19">
         <v>512</v>
       </c>
-      <c r="G10" s="24"/>
-      <c r="H10" s="23">
+      <c r="G10" s="20"/>
+      <c r="H10" s="19">
         <v>256</v>
       </c>
-      <c r="I10" s="23">
+      <c r="I10" s="19">
         <v>512</v>
       </c>
-      <c r="J10" s="23">
+      <c r="J10" s="19">
         <v>1024</v>
       </c>
-      <c r="K10" s="23">
+      <c r="K10" s="19">
         <v>256</v>
       </c>
-      <c r="L10" s="23">
+      <c r="L10" s="19">
         <v>512</v>
       </c>
-      <c r="M10" s="23">
+      <c r="M10" s="19">
         <v>256</v>
       </c>
-      <c r="N10" s="23">
+      <c r="N10" s="19">
         <v>256</v>
       </c>
-      <c r="O10" s="23">
+      <c r="O10" s="19">
         <v>256</v>
       </c>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="24"/>
-      <c r="R10" s="23">
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="19">
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="2:18" s="25" customFormat="1">
-      <c r="B11" s="31" t="s">
+    <row r="11" spans="2:18" s="21" customFormat="1">
+      <c r="B11" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="23" t="s">
+      <c r="C11" s="39"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="I11" s="23" t="s">
+      <c r="I11" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="J11" s="23" t="s">
+      <c r="J11" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="K11" s="23" t="s">
+      <c r="K11" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="L11" s="23" t="s">
+      <c r="L11" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="M11" s="23" t="s">
+      <c r="M11" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="N11" s="23" t="s">
+      <c r="N11" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="O11" s="23" t="s">
+      <c r="O11" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="23" t="s">
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="19" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="2:18" s="25" customFormat="1">
-      <c r="B12" s="31" t="s">
+    <row r="12" spans="2:18" s="21" customFormat="1">
+      <c r="B12" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="34" t="s">
+      <c r="C12" s="39"/>
+      <c r="D12" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="E12" s="34" t="s">
+      <c r="E12" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="F12" s="34" t="s">
+      <c r="F12" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="G12" s="34" t="s">
+      <c r="G12" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="H12" s="23" t="s">
+      <c r="H12" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="I12" s="23" t="s">
+      <c r="I12" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="J12" s="23" t="s">
+      <c r="J12" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="K12" s="23" t="s">
+      <c r="K12" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="L12" s="23" t="s">
+      <c r="L12" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="M12" s="23" t="s">
+      <c r="M12" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="N12" s="23" t="s">
+      <c r="N12" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="O12" s="23" t="s">
+      <c r="O12" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="23" t="s">
+      <c r="P12" s="20"/>
+      <c r="Q12" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="R12" s="23" t="s">
+      <c r="R12" s="19" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="2:18" s="25" customFormat="1">
-      <c r="B13" s="9" t="s">
+    <row r="13" spans="2:18" s="21" customFormat="1">
+      <c r="B13" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="23" t="s">
+      <c r="C13" s="34"/>
+      <c r="D13" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="23" t="s">
+      <c r="F13" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="G13" s="23" t="s">
+      <c r="G13" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="H13" s="23" t="s">
+      <c r="H13" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="I13" s="23" t="s">
+      <c r="I13" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="J13" s="23" t="s">
+      <c r="J13" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="K13" s="23" t="s">
+      <c r="K13" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23" t="s">
+      <c r="L13" s="19"/>
+      <c r="M13" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="N13" s="23" t="s">
+      <c r="N13" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="O13" s="23" t="s">
+      <c r="O13" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="P13" s="24"/>
-      <c r="Q13" s="24"/>
-      <c r="R13" s="23" t="s">
+      <c r="P13" s="20"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="19" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="2:18" s="25" customFormat="1" ht="30">
-      <c r="B14" s="9" t="s">
+    <row r="14" spans="2:18" s="21" customFormat="1" ht="30">
+      <c r="B14" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="26" t="s">
+      <c r="D14" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="26" t="s">
+      <c r="E14" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="G14" s="24"/>
-      <c r="H14" s="23" t="s">
+      <c r="G14" s="20"/>
+      <c r="H14" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="I14" s="23" t="s">
+      <c r="I14" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="23" t="s">
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="M14" s="24"/>
-      <c r="N14" s="24"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="24"/>
-      <c r="R14" s="24"/>
-    </row>
-    <row r="15" spans="2:18" s="17" customFormat="1" ht="90">
-      <c r="B15" s="9"/>
-      <c r="C15" s="12" t="s">
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="20"/>
+    </row>
+    <row r="15" spans="2:18" s="13" customFormat="1" ht="90">
+      <c r="B15" s="34"/>
+      <c r="C15" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="26">
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="22">
         <v>100</v>
       </c>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="26">
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="22">
         <v>100</v>
       </c>
-      <c r="K15" s="26">
+      <c r="K15" s="22">
         <v>100</v>
       </c>
-      <c r="L15" s="39"/>
-      <c r="M15" s="19" t="s">
+      <c r="L15" s="31"/>
+      <c r="M15" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="N15" s="19" t="s">
+      <c r="N15" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="O15" s="19" t="s">
+      <c r="O15" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="P15" s="39"/>
-      <c r="Q15" s="39"/>
-      <c r="R15" s="19" t="s">
+      <c r="P15" s="31"/>
+      <c r="Q15" s="31"/>
+      <c r="R15" s="15" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="16" spans="2:18" s="17" customFormat="1" ht="45">
-      <c r="B16" s="9" t="s">
+    <row r="16" spans="2:18" s="13" customFormat="1" ht="45">
+      <c r="B16" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="26" t="s">
+      <c r="C16" s="34"/>
+      <c r="D16" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="26" t="s">
+      <c r="E16" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="F16" s="26" t="s">
+      <c r="F16" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="G16" s="39"/>
-      <c r="H16" s="26" t="s">
+      <c r="G16" s="31"/>
+      <c r="H16" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="I16" s="26" t="s">
+      <c r="I16" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="J16" s="26" t="s">
+      <c r="J16" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="K16" s="26" t="s">
+      <c r="K16" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="L16" s="26" t="s">
+      <c r="L16" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="M16" s="26" t="s">
+      <c r="M16" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="N16" s="26" t="s">
+      <c r="N16" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="O16" s="26" t="s">
+      <c r="O16" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="P16" s="39"/>
-      <c r="Q16" s="39"/>
-      <c r="R16" s="19" t="s">
+      <c r="P16" s="31"/>
+      <c r="Q16" s="31"/>
+      <c r="R16" s="15" t="s">
         <v>124</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="M4:R4"/>
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="H4:L4"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
ajout CQ CE dans les tableaux
</commit_message>
<xml_diff>
--- a/Synthèse.xlsx
+++ b/Synthèse.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="144">
   <si>
     <t>Tension (kV)</t>
   </si>
@@ -142,13 +142,7 @@
     <t>Nombre de coups (kcp)</t>
   </si>
   <si>
-    <t>Durée (s)</t>
-  </si>
-  <si>
     <t>Contrôle</t>
-  </si>
-  <si>
-    <t>Type</t>
   </si>
   <si>
     <t>Intrinséque</t>
@@ -267,9 +261,6 @@
     </r>
   </si>
   <si>
-    <t>Mode Planaire</t>
-  </si>
-  <si>
     <t>Test visuel:
 non uniformité
 spectrométrie
@@ -371,9 +362,6 @@
 Puis Galette de Co57</t>
   </si>
   <si>
-    <t>Mode Tomographique</t>
-  </si>
-  <si>
     <t>Determination du centre de rotation</t>
   </si>
   <si>
@@ -442,15 +430,6 @@
 Taille pixel= (distance entre 2 lignes/Nb pixel entre 2 ligne)</t>
   </si>
   <si>
-    <t>25 s par projection
-120 projections
-réalisées dans le sens horaire</t>
-  </si>
-  <si>
-    <t>10 s par pas d'acquisition
-1 acquisition tous les 6° sur 720° réalisation des acquisition dans le sens horraire</t>
-  </si>
-  <si>
     <t>Contrôle non réalisé.</t>
   </si>
   <si>
@@ -470,10 +449,6 @@
     <t>140 ± 20%
 et
 120 ± 10%</t>
-  </si>
-  <si>
-    <t>15 s / projection
-30 projections /détecteur</t>
   </si>
   <si>
     <t>Acquisition d'un fantôme QI adaptés à la MN (Jaszszak).
@@ -482,6 +457,97 @@
 Contraste
 Bruit
 …</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>Planaire</t>
+  </si>
+  <si>
+    <t>Tomographique</t>
+  </si>
+  <si>
+    <t>Corps Entier</t>
+  </si>
+  <si>
+    <t>Variation longitudinal de la spectrométrie</t>
+  </si>
+  <si>
+    <t>Non-unifrmité de réponse du système</t>
+  </si>
+  <si>
+    <t>- Initial
+- Annuel
+- En cas de défaut du mode balayage en mode CE</t>
+  </si>
+  <si>
+    <t>- A Réception</t>
+  </si>
+  <si>
+    <t>Ecart max position du pic &lt; 2 keV
+± 1 % / CQ Initial</t>
+  </si>
+  <si>
+    <t>Ansence de défauts sur l'image</t>
+  </si>
+  <si>
+    <t>Degradation RE CE &lt; 10% / RS Planaire</t>
+  </si>
+  <si>
+    <t>Source de Co 57 sur le détecteur sous la table
+Acquisition pour 3 position de table
+PAS D'INTERET QUAND BALAYAGE PAS MOUVEMENT DE TABLE</t>
+  </si>
+  <si>
+    <t>Co 57</t>
+  </si>
+  <si>
+    <t>11 min
+Balayage continu sur 199 cm
+à 18 cm/min</t>
+  </si>
+  <si>
+    <t>Durée</t>
+  </si>
+  <si>
+    <t>100 s</t>
+  </si>
+  <si>
+    <t>20 min
+10 s par pas d'acquisition
+1 acquisition tous les 6° sur 720° réalisation des acquisition dans le sens horraire</t>
+  </si>
+  <si>
+    <t>50 min
+25 s par projection
+120 projections
+réalisées dans le sens horaire</t>
+  </si>
+  <si>
+    <t>8 min
+15 s / projection
+30 projections /détecteur</t>
+  </si>
+  <si>
+    <t>Source de Co 57 sur le détecteur sous la table
+Acquisition d'un balayage CE</t>
+  </si>
+  <si>
+    <t>Balayage CE</t>
+  </si>
+  <si>
+    <t>5 min
+Balayage continu sur 80 cm
+à 18 cm/min</t>
+  </si>
+  <si>
+    <t>256 x 1024</t>
+  </si>
+  <si>
+    <t>Ligne source Tc 99m
+distance source détecteur 15 cm pour les deux détécteur
+détermination des LMH en X (direction de balayage) et Y(direction perpendiculaire au balayage)</t>
   </si>
 </sst>
 </file>
@@ -540,7 +606,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -586,6 +652,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -640,7 +718,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -698,8 +776,26 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -814,8 +910,17 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="75">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -844,6 +949,15 @@
     <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -872,6 +986,15 @@
     <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1547,13 +1670,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:R16"/>
+  <dimension ref="B1:U16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="O6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="Q9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="S9" sqref="S9"/>
+      <selection pane="bottomRight" activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1568,292 +1691,345 @@
     <col min="8" max="12" width="25.5" style="12" customWidth="1"/>
     <col min="13" max="17" width="21.5" style="12" customWidth="1"/>
     <col min="18" max="18" width="22.33203125" style="12" customWidth="1"/>
-    <col min="19" max="16384" width="10.83203125" style="12"/>
+    <col min="19" max="19" width="22.83203125" style="12" customWidth="1"/>
+    <col min="20" max="20" width="22.5" style="12" customWidth="1"/>
+    <col min="21" max="21" width="23.33203125" style="12" customWidth="1"/>
+    <col min="22" max="16384" width="10.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18">
+    <row r="1" spans="2:21">
       <c r="B1" s="35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" s="35"/>
     </row>
-    <row r="4" spans="2:18" s="4" customFormat="1">
+    <row r="4" spans="2:21" s="4" customFormat="1">
       <c r="B4" s="34" t="s">
-        <v>41</v>
+        <v>120</v>
       </c>
       <c r="C4" s="34"/>
       <c r="D4" s="33" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E4" s="33"/>
       <c r="F4" s="33"/>
       <c r="G4" s="33"/>
       <c r="H4" s="37" t="s">
-        <v>69</v>
+        <v>121</v>
       </c>
       <c r="I4" s="37"/>
       <c r="J4" s="37"/>
       <c r="K4" s="37"/>
       <c r="L4" s="37"/>
       <c r="M4" s="32" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="N4" s="32"/>
       <c r="O4" s="32"/>
       <c r="P4" s="32"/>
       <c r="Q4" s="32"/>
       <c r="R4" s="32"/>
-    </row>
-    <row r="5" spans="2:18" s="8" customFormat="1" ht="60">
+      <c r="S4" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="T4" s="40"/>
+      <c r="U4" s="40"/>
+    </row>
+    <row r="5" spans="2:21" s="8" customFormat="1" ht="60">
       <c r="B5" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="36"/>
       <c r="D5" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="G5" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="H5" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="K5" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="L5" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="N5" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="O5" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="P5" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q5" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="R5" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="S5" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="T5" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="U5" s="41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" s="14" customFormat="1">
+      <c r="B6" s="36" t="s">
         <v>45</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="I5" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="J5" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="K5" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="L5" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="M5" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="N5" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="O5" s="28" t="s">
-        <v>99</v>
-      </c>
-      <c r="P5" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q5" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="R5" s="28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="2:18" s="14" customFormat="1">
-      <c r="B6" s="36" t="s">
-        <v>47</v>
       </c>
       <c r="C6" s="36"/>
       <c r="D6" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F6" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="M6" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="N6" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="O6" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="P6" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q6" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="R6" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="S6" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="T6" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="U6" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" s="14" customFormat="1" ht="75">
+      <c r="B7" s="36" t="s">
         <v>48</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="L6" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="M6" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="N6" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="O6" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="P6" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q6" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="R6" s="15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="2:18" s="14" customFormat="1" ht="75">
-      <c r="B7" s="36" t="s">
-        <v>50</v>
       </c>
       <c r="C7" s="36"/>
       <c r="D7" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G7" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="H7" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="M7" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="N7" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="P7" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q7" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="H7" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="J7" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="K7" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="L7" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="M7" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="N7" s="16" t="s">
+      <c r="R7" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="O7" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="P7" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q7" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="R7" s="16" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="2:18" s="18" customFormat="1" ht="60">
+      <c r="S7" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="T7" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="U7" s="42" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" s="18" customFormat="1" ht="60">
       <c r="B8" s="36" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C8" s="36"/>
       <c r="D8" s="17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H8" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="I8" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="J8" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="K8" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="L8" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="J8" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="K8" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="L8" s="17" t="s">
-        <v>82</v>
-      </c>
       <c r="M8" s="24" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="N8" s="24" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="O8" s="30"/>
       <c r="P8" s="30"/>
       <c r="Q8" s="24" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="R8" s="30"/>
-    </row>
-    <row r="9" spans="2:18" s="18" customFormat="1" ht="127" customHeight="1">
+      <c r="S8" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="T8" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="U8" s="24" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" s="18" customFormat="1" ht="142" customHeight="1">
       <c r="B9" s="36" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C9" s="36"/>
       <c r="D9" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>67</v>
-      </c>
       <c r="H9" s="24" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J9" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="K9" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="K9" s="24" t="s">
-        <v>95</v>
-      </c>
       <c r="L9" s="24" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="M9" s="24" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="N9" s="24" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="O9" s="24" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="P9" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q9" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="R9" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="Q9" s="24" t="s">
-        <v>123</v>
-      </c>
-      <c r="R9" s="24" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="10" spans="2:18" s="21" customFormat="1">
+      <c r="S9" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="T9" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="U9" s="24" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" s="21" customFormat="1">
       <c r="B10" s="34" t="s">
         <v>35</v>
       </c>
@@ -1897,10 +2073,17 @@
       <c r="R10" s="19">
         <v>128</v>
       </c>
-    </row>
-    <row r="11" spans="2:18" s="21" customFormat="1">
+      <c r="S10" s="20"/>
+      <c r="T10" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="U10" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" s="21" customFormat="1">
       <c r="B11" s="38" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C11" s="39"/>
       <c r="D11" s="26"/>
@@ -1908,130 +2091,157 @@
       <c r="F11" s="26"/>
       <c r="G11" s="26"/>
       <c r="H11" s="19" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I11" s="19" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J11" s="19" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="K11" s="19" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="L11" s="19" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M11" s="19" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="N11" s="19" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="O11" s="19" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="P11" s="20"/>
       <c r="Q11" s="20"/>
       <c r="R11" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="S11" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="T11" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="U11" s="19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" s="21" customFormat="1">
+      <c r="B12" s="38" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="2:18" s="21" customFormat="1">
-      <c r="B12" s="38" t="s">
-        <v>87</v>
       </c>
       <c r="C12" s="39"/>
       <c r="D12" s="27" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G12" s="27" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H12" s="19" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I12" s="19" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="J12" s="19" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K12" s="19" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="L12" s="19" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="M12" s="19" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="N12" s="19" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="O12" s="19" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="P12" s="20"/>
       <c r="Q12" s="19" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="R12" s="19" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="2:18" s="21" customFormat="1">
+        <v>91</v>
+      </c>
+      <c r="S12" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="T12" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="U12" s="19" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" s="21" customFormat="1">
       <c r="B13" s="34" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="34"/>
       <c r="D13" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G13" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H13" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I13" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J13" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K13" s="19" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="L13" s="19"/>
       <c r="M13" s="19" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="N13" s="19" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="O13" s="19" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="P13" s="20"/>
       <c r="Q13" s="20"/>
       <c r="R13" s="19" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="14" spans="2:18" s="21" customFormat="1" ht="30">
+        <v>110</v>
+      </c>
+      <c r="S13" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="T13" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="U13" s="19" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" s="21" customFormat="1" ht="30">
       <c r="B14" s="34" t="s">
         <v>37</v>
       </c>
@@ -2039,25 +2249,25 @@
         <v>38</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G14" s="20"/>
       <c r="H14" s="19" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I14" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J14" s="20"/>
       <c r="K14" s="20"/>
       <c r="L14" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="M14" s="20"/>
       <c r="N14" s="20"/>
@@ -2065,89 +2275,111 @@
       <c r="P14" s="20"/>
       <c r="Q14" s="20"/>
       <c r="R14" s="20"/>
-    </row>
-    <row r="15" spans="2:18" s="13" customFormat="1" ht="90">
+      <c r="S14" s="22">
+        <v>500</v>
+      </c>
+      <c r="T14" s="20"/>
+      <c r="U14" s="20"/>
+    </row>
+    <row r="15" spans="2:21" s="13" customFormat="1" ht="105">
       <c r="B15" s="34"/>
       <c r="C15" s="10" t="s">
-        <v>39</v>
+        <v>134</v>
       </c>
       <c r="D15" s="31"/>
       <c r="E15" s="31"/>
       <c r="F15" s="31"/>
-      <c r="G15" s="22">
-        <v>100</v>
+      <c r="G15" s="22" t="s">
+        <v>135</v>
       </c>
       <c r="H15" s="31"/>
       <c r="I15" s="31"/>
-      <c r="J15" s="22">
-        <v>100</v>
-      </c>
-      <c r="K15" s="22">
-        <v>100</v>
+      <c r="J15" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="K15" s="22" t="s">
+        <v>135</v>
       </c>
       <c r="L15" s="31"/>
       <c r="M15" s="15" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="N15" s="15" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
       <c r="O15" s="15" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
       <c r="P15" s="31"/>
       <c r="Q15" s="31"/>
       <c r="R15" s="15" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="16" spans="2:18" s="13" customFormat="1" ht="45">
+        <v>138</v>
+      </c>
+      <c r="S15" s="31"/>
+      <c r="T15" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="U15" s="15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" s="13" customFormat="1" ht="45">
       <c r="B16" s="34" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C16" s="34"/>
       <c r="D16" s="22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G16" s="31"/>
       <c r="H16" s="22" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I16" s="22" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J16" s="22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K16" s="22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L16" s="22" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="M16" s="22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="N16" s="22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="O16" s="22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="P16" s="31"/>
       <c r="Q16" s="31"/>
       <c r="R16" s="15" t="s">
-        <v>124</v>
+        <v>118</v>
+      </c>
+      <c r="S16" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="T16" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="U16" s="22" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="17">
+    <mergeCell ref="S4:U4"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="B16:C16"/>
@@ -2166,6 +2398,7 @@
     <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>